<commit_message>
Now done FOR REAL
</commit_message>
<xml_diff>
--- a/lab_4/PSP.xlsx
+++ b/lab_4/PSP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ugniu\code\algorithms_and_data_structures\lab_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00ABBE98-DEBB-45D6-9FA3-1105E628E698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5A6D4A-8677-41D0-A847-3742609EB95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LFF" sheetId="8" r:id="rId1"/>
@@ -743,7 +743,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="168">
   <si>
     <t>Data</t>
   </si>
@@ -1263,6 +1263,9 @@
   </si>
   <si>
     <t>Grafai</t>
+  </si>
+  <si>
+    <t>2025.05.13</t>
   </si>
 </sst>
 </file>
@@ -1852,11 +1855,38 @@
     <xf numFmtId="166" fontId="23" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1864,37 +1894,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -2262,8 +2265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8665FC0F-487C-4E54-BDED-849B77F1CD73}">
   <dimension ref="A2:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2416,10 +2419,10 @@
         <v>150</v>
       </c>
       <c r="C7" s="84">
-        <v>0.5</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D7" s="84">
-        <v>0.58333333333333337</v>
+        <v>0.125</v>
       </c>
       <c r="E7" s="83">
         <v>0</v>
@@ -2445,10 +2448,10 @@
         <v>150</v>
       </c>
       <c r="C8" s="82">
-        <v>0.63541666666666663</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="D8" s="82">
-        <v>0.64236111111111116</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="E8" s="81">
         <v>0</v>
@@ -2468,7 +2471,7 @@
     <row r="9" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="63"/>
       <c r="B9" s="83" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="C9" s="82">
         <v>0.42708333333333331</v>
@@ -2793,11 +2796,11 @@
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="97" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2829,10 +2832,10 @@
       <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="92" t="s">
+      <c r="C5" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="92"/>
+      <c r="D5" s="99"/>
       <c r="E5" s="6" t="s">
         <v>21</v>
       </c>
@@ -2843,10 +2846,10 @@
       <c r="B6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="93" t="s">
+      <c r="C6" s="87" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="94"/>
+      <c r="D6" s="92"/>
       <c r="E6" s="8">
         <v>0</v>
       </c>
@@ -2854,10 +2857,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="89"/>
+      <c r="B7" s="93"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="95"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2865,10 +2868,10 @@
       <c r="B8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="93" t="s">
+      <c r="C8" s="87" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="95"/>
+      <c r="D8" s="88"/>
       <c r="E8" s="8">
         <v>0</v>
       </c>
@@ -2876,10 +2879,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="87"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="89"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="95"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2887,10 +2890,10 @@
       <c r="B10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="93" t="s">
+      <c r="C10" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="95"/>
+      <c r="D10" s="88"/>
       <c r="E10" s="8">
         <v>0</v>
       </c>
@@ -2898,10 +2901,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="87"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="89"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="95"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2909,10 +2912,10 @@
       <c r="B12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="93" t="s">
+      <c r="C12" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="95"/>
+      <c r="D12" s="88"/>
       <c r="E12" s="8">
         <v>0</v>
       </c>
@@ -2920,10 +2923,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="89"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="95"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2931,10 +2934,10 @@
       <c r="B14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="96" t="s">
+      <c r="C14" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="97"/>
+      <c r="D14" s="101"/>
       <c r="E14" s="8">
         <v>0</v>
       </c>
@@ -2942,10 +2945,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="89"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="95"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -2953,19 +2956,19 @@
       <c r="B16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="93" t="s">
+      <c r="C16" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="94"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="8"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="87"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="89"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="95"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2973,10 +2976,10 @@
       <c r="B18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="93" t="s">
+      <c r="C18" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="94"/>
+      <c r="D18" s="92"/>
       <c r="E18" s="8">
         <v>0</v>
       </c>
@@ -2984,10 +2987,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="89"/>
+      <c r="B19" s="93"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="95"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2995,10 +2998,10 @@
       <c r="B20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="94"/>
+      <c r="D20" s="92"/>
       <c r="E20" s="8">
         <v>0</v>
       </c>
@@ -3006,10 +3009,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="87"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="89"/>
+      <c r="B21" s="93"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="95"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
@@ -3017,10 +3020,10 @@
       <c r="B22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="93" t="s">
+      <c r="C22" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="95"/>
+      <c r="D22" s="88"/>
       <c r="E22" s="8">
         <v>0</v>
       </c>
@@ -3028,11 +3031,11 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="98" t="s">
+      <c r="B23" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="99"/>
-      <c r="D23" s="100"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="91"/>
       <c r="E23" s="11">
         <f>SUM(E6:E22)</f>
         <v>0</v>
@@ -3049,14 +3052,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B21:E21"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C5:D5"/>
@@ -3069,6 +3064,14 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3584,7 +3587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB68080-A135-4866-A00B-24DFED103D03}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>